<commit_message>
add testcase about LTC
</commit_message>
<xml_diff>
--- a/test/testcase/Wanchain RPC API Testcase.xlsx
+++ b/test/testcase/Wanchain RPC API Testcase.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="1050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="1104">
   <si>
     <t>ProgramName</t>
   </si>
@@ -9585,6 +9585,351 @@
   </si>
   <si>
     <t>TC6033</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7001</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>LTC</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>getUTXO</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get UTXOs of address</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "automate tests",
+        "method": "getUTXO",
+        "params": {
+          "chainType": "LTC",
+          "minconf": 0,
+          "maxconf": 1000000,
+          "address": ["n1Z6fZEkmMo9Uy9tSdE9L3CSn5jhc7eYzH"]
+    }
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "automate tests",
+  "result": [{"txid":"33702f8915d36c812f9e0deed0bae5e5d216a615db4bd0b9b5746944fcc2baf5","vout":1,"address":"n1Z6fZEkmMo9Uy9tSdE9L3CSn5jhc7eYzH","label":"","scriptPubKey":"76a914dbca55cb819d9bb66f452e7bdc0554e23ff2144488ac","amount":1.6451565,"confirmations":32,"spendable":false,"solvable":false,"safe":true,"value":1.6451565}]
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7002</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>getTxInfo</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get Tx info with hex string</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "user defined field",
+        "method": "getTxInfo",
+        "params": {
+          "chainType": "LTC",
+          "txHash": "70f22d78a3657d6ec5a6fb6d59e59b860ee9aa7e2e0ee1a31d39a5d0423f8e59"
+        }
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "result": "020000000001010000000000000000000000000000000000000000000000000000000000000000ffffffff0603cef41c0101ffffffff02807c814a0000000017a91411fb66e35a4d3b7c548fff18683fdd2262b5a080870000000000000000266a24aa21a9ede2f61c3f71d1defd3fa999dfa36953755c690689799962b48bebd836974e8cf90120000000000000000000000000000000000000000000000000000000000000000000000000"
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7003</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get Tx info with json type.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "user defined field",
+        "method": "getTxInfo",
+        "params": {
+          "chainType":"LTC","format":true,
+         "txHash":"70f22d78a3657d6ec5a6fb6d59e59b860ee9aa7e2e0ee1a31d39a5d0423f8e59"
+        }
+      }</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "result": {"txid":"70f22d78a3657d6ec5a6fb6d59e59b860ee9aa7e2e0ee1a31d39a5d0423f8e59","hash":"9100a27eeef89558f69cfa87bd5dec1be412aeffd12a0685a5f6ad3ae51f1aa4","version":2,"size":172,"vsize":145,"weight":580,"locktime":0,"vin":[{"coinbase":"03cef41c0101","sequence":4294967295}],"vout":[{"value":12.5,"n":0,"scriptPubKey":{"asm":"OP_HASH160 11fb66e35a4d3b7c548fff18683fdd2262b5a080 OP_EQUAL","hex":"a91411fb66e35a4d3b7c548fff18683fdd2262b5a08087","reqSigs":1,"type":"scripthash","addresses":["QNF4mGeum2B5a1YyuLXJVKyEWaNgnezeaG"]}},{"value":0,"n":1,"scriptPubKey":{"asm":"OP_RETURN aa21a9ede2f61c3f71d1defd3fa999dfa36953755c690689799962b48bebd836974e8cf9","hex":"6a24aa21a9ede2f61c3f71d1defd3fa999dfa36953755c690689799962b48bebd836974e8cf9","type":"nulldata"}}],"hex":"020000000001010000000000000000000000000000000000000000000000000000000000000000ffffffff0603cef41c0101ffffffff02807c814a0000000017a91411fb66e35a4d3b7c548fff18683fdd2262b5a080870000000000000000266a24aa21a9ede2f61c3f71d1defd3fa999dfa36953755c690689799962b48bebd836974e8cf90120000000000000000000000000000000000000000000000000000000000000000000000000","blockhash":"69f2f172fa220e355f9db8a394db979b38099dfe89a095755d98b14f1a00117b","confirmations":4708,"time":1620960052,"blocktime":1620960052}
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7004</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>sendRawTransaction</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send raw transaction</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+ "id": "user defined field",
+ "method": "sendRawTransaction",
+ "params": {
+"chainType":"LTC",
+"signedTx":"0100000001519f23f7e55d5a0e6b08be4ef64feb79eb4f97e52fc27d4b68ec878961ed18f100000000ec483045022100f2c54d35ff53839d9142a6bcbb3e9ea4773e67a40f993afb09c2e4b8b49c91eb022039928104f097d33730699e98316ca4b0663cef7fdb0feea8377eee9acb0f01f5012102e2bcce70a6125b37e5feb2100c70accd45981908e211e71e8a4805998893d41520800f8294162d6f7e40463c26891670c85aab09ec5487ac5c5de4ae0afd6a92e2514c5d63a8208ff1c9ec2d395066456858c6a0c38ad07bac7b4768885fc9a3b983ace9148d758876a9143390865291090a98c6eda2ff3868383d4d7af175670441a4865bb17576a914d3a80a8e8bf8fbfea8eee3193dc834e61f257dfe6888acffffffff0180841e00000000001976a9143390865291090a98c6eda2ff3868383d4d7af17588ac00000000"
+        }
+      }</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "error": "Missing inputs"
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7005</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>importAddress</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Import ltc address to node.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "user defined field",
+        "method": "importAddress",
+        "params": {
+          "chainType":"LTC",
+    "address":"n1Z6fZEkmMo9Uy9tSdE9L3CSn5jhc7eYzH"}
+      }</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "result":"success"
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7006</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>estimateSmartFee</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>estimate smart fee from node.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "user defined field",
+        "method": "estimateSmartFee",
+        "params": {
+          "chainType":"LTC"
+        }
+      }</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "result":49
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7007</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>estimateNetworkFee</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>estimate network lock fee from node.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "user defined field",
+        "method": "estimateNetworkFee",
+        "params": {
+          "chainType":"LTC",
+          "feeType":"lock"
+        }
+      }</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "result":"0"
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7008</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>estimate network release fee from node.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "user defined field",
+        "method": "estimateNetworkFee",
+        "params": {
+          "chainType":"LTC",
+          "feeType":"release"
+        }
+      }</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7009</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>getCrossChainFees</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>get cross chain fees.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "user defined field",
+        "method": "getCrossChainFees",
+        "params": {
+          "chainType":"LTC",
+          "chainIds":["0x80000002", "0x8000003c"]
+        }
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "result":{"lockFee":"0","revokeFee":"0"}
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7010</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>getBlockNumber</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>get current block height.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "user defined field",
+        "method": "getBlockNumber",
+        "params": {
+          "chainType":"LTC"
+        }
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "result":1902404
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC7011</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>LTC</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>getUTXO</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>get utxo with WAN address.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+ "jsonrpc": "2.0",
+        "id": "automate tests",
+        "method": "getUTXO",
+        "params": {
+          "chainType": "LTC",
+          "minconf": 0,
+          "maxconf": 1000000,
+          "address": ["0x9d52EC3478cccA75b1BBb0EFaFBD01edb276253d"]
+    }
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "jsonrpc": "2.0",
+  "id": "user defined field",
+  "error":"Invalid address"
+}</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -10032,7 +10377,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -10361,13 +10706,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O253"/>
+  <dimension ref="A1:O264"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D263" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A162" sqref="A162"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="F264" sqref="F264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -17422,6 +17767,314 @@
         <v>93</v>
       </c>
       <c r="J253" s="6"/>
+    </row>
+    <row r="254" spans="1:10" ht="147" customHeight="1">
+      <c r="A254" s="13" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B254" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C254" s="4" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D254" s="6" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E254" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F254" s="6" t="s">
+        <v>1054</v>
+      </c>
+      <c r="G254" s="7" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H254" s="4"/>
+      <c r="I254" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J254" s="6"/>
+    </row>
+    <row r="255" spans="1:10" ht="147" customHeight="1">
+      <c r="A255" s="13" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B255" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C255" s="4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D255" s="6" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E255" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F255" s="6" t="s">
+        <v>1059</v>
+      </c>
+      <c r="G255" s="7" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H255" s="4"/>
+      <c r="I255" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J255" s="6"/>
+    </row>
+    <row r="256" spans="1:10" ht="147" customHeight="1">
+      <c r="A256" s="13" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B256" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C256" s="4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D256" s="6" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E256" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F256" s="6" t="s">
+        <v>1063</v>
+      </c>
+      <c r="G256" s="7" t="s">
+        <v>1064</v>
+      </c>
+      <c r="H256" s="4"/>
+      <c r="I256" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J256" s="6"/>
+    </row>
+    <row r="257" spans="1:10" ht="147" customHeight="1">
+      <c r="A257" s="13" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B257" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C257" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D257" s="6" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E257" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F257" s="6" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G257" s="7" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H257" s="4"/>
+      <c r="I257" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="J257" s="6"/>
+    </row>
+    <row r="258" spans="1:10" ht="147" customHeight="1">
+      <c r="A258" s="13" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B258" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C258" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D258" s="6" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E258" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F258" s="6" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G258" s="7" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H258" s="4"/>
+      <c r="I258" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J258" s="6"/>
+    </row>
+    <row r="259" spans="1:10" ht="147" customHeight="1">
+      <c r="A259" s="13" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B259" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C259" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D259" s="6" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E259" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F259" s="6" t="s">
+        <v>1078</v>
+      </c>
+      <c r="G259" s="7" t="s">
+        <v>1079</v>
+      </c>
+      <c r="H259" s="4"/>
+      <c r="I259" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J259" s="6"/>
+    </row>
+    <row r="260" spans="1:10" ht="147" customHeight="1">
+      <c r="A260" s="13" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B260" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C260" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D260" s="6" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E260" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F260" s="6" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G260" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="H260" s="4"/>
+      <c r="I260" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J260" s="6"/>
+    </row>
+    <row r="261" spans="1:10" ht="147" customHeight="1">
+      <c r="A261" s="13" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B261" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C261" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D261" s="6" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E261" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F261" s="6" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G261" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="H261" s="4"/>
+      <c r="I261" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J261" s="6"/>
+    </row>
+    <row r="262" spans="1:10" ht="147" customHeight="1">
+      <c r="A262" s="13" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B262" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C262" s="4" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D262" s="6" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E262" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F262" s="6" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G262" s="7" t="s">
+        <v>1092</v>
+      </c>
+      <c r="H262" s="4"/>
+      <c r="I262" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J262" s="6"/>
+    </row>
+    <row r="263" spans="1:10" ht="147" customHeight="1">
+      <c r="A263" s="13" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B263" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C263" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D263" s="6" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E263" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F263" s="6" t="s">
+        <v>1096</v>
+      </c>
+      <c r="G263" s="7" t="s">
+        <v>1097</v>
+      </c>
+      <c r="H263" s="4"/>
+      <c r="I263" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J263" s="6"/>
+    </row>
+    <row r="264" spans="1:10" ht="147" customHeight="1">
+      <c r="A264" s="13" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C264" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D264" s="6" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E264" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F264" s="6" t="s">
+        <v>1102</v>
+      </c>
+      <c r="G264" s="7" t="s">
+        <v>1103</v>
+      </c>
+      <c r="H264" s="4"/>
+      <c r="I264" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J264" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>